<commit_message>
BIS-769: Fixed test after merge
</commit_message>
<xml_diff>
--- a/server-application-server/sourceTest/java/ch/ethz/sis/openbis/generic/server/xls/export/resources/export-sample-with-referred-types.xlsx
+++ b/server-application-server/sourceTest/java/ch/ethz/sis/openbis/generic/server/xls/export/resources/export-sample-with-referred-types.xlsx
@@ -8,7 +8,7 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="73">
   <si>
     <t xml:space="preserve">SAMPLE_TYPE</t>
   </si>
@@ -86,6 +86,12 @@
   </si>
   <si>
     <t xml:space="preserve">Unique</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pattern</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pattern Type</t>
   </si>
   <si>
     <t xml:space="preserve">$NAME</t>
@@ -465,124 +471,18 @@
 </styleSheet>
 </file>
 
-<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office Theme">
-  <a:themeElements>
-    <a:clrScheme name="LibreOffice">
-      <a:dk1>
-        <a:srgbClr val="000000"/>
-      </a:dk1>
-      <a:lt1>
-        <a:srgbClr val="ffffff"/>
-      </a:lt1>
-      <a:dk2>
-        <a:srgbClr val="000000"/>
-      </a:dk2>
-      <a:lt2>
-        <a:srgbClr val="ffffff"/>
-      </a:lt2>
-      <a:accent1>
-        <a:srgbClr val="18a303"/>
-      </a:accent1>
-      <a:accent2>
-        <a:srgbClr val="0369a3"/>
-      </a:accent2>
-      <a:accent3>
-        <a:srgbClr val="a33e03"/>
-      </a:accent3>
-      <a:accent4>
-        <a:srgbClr val="8e03a3"/>
-      </a:accent4>
-      <a:accent5>
-        <a:srgbClr val="c99c00"/>
-      </a:accent5>
-      <a:accent6>
-        <a:srgbClr val="c9211e"/>
-      </a:accent6>
-      <a:hlink>
-        <a:srgbClr val="0000ee"/>
-      </a:hlink>
-      <a:folHlink>
-        <a:srgbClr val="551a8b"/>
-      </a:folHlink>
-    </a:clrScheme>
-    <a:fontScheme name="Office">
-      <a:majorFont>
-        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
-        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
-        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
-      </a:majorFont>
-      <a:minorFont>
-        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
-        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
-        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
-      </a:minorFont>
-    </a:fontScheme>
-    <a:fmtScheme>
-      <a:fillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:fillStyleLst>
-      <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:prstDash val="solid"/>
-          <a:miter/>
-        </a:ln>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:prstDash val="solid"/>
-          <a:miter/>
-        </a:ln>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:prstDash val="solid"/>
-          <a:miter/>
-        </a:ln>
-      </a:lnStyleLst>
-      <a:effectStyleLst>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-      </a:effectStyleLst>
-      <a:bgFillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:bgFillStyleLst>
-    </a:fmtScheme>
-  </a:themeElements>
-</a:theme>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMN1048576"/>
+  <dimension ref="A1:Q1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E10" activeCellId="0" sqref="E10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="N13" activeCellId="0" sqref="N13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.51171875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.51953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="38.68"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="42.5"/>
@@ -595,8 +495,6 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="18.19"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="9.21"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="18.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1026" min="1026" style="1" width="8.36"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16383" style="1" width="8.37"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -683,29 +581,35 @@
       <c r="L4" s="6" t="s">
         <v>21</v>
       </c>
+      <c r="M4" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="N4" s="6" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>10</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="G5" s="4"/>
       <c r="H5" s="4" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="I5" s="4"/>
       <c r="J5" s="4"/>
@@ -718,26 +622,26 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>10</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="G6" s="4"/>
       <c r="H6" s="4" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="I6" s="4"/>
       <c r="J6" s="4"/>
@@ -778,10 +682,10 @@
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>10</v>
@@ -832,29 +736,35 @@
       <c r="L11" s="6" t="s">
         <v>21</v>
       </c>
+      <c r="M11" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="N11" s="6" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="4" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>10</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="G12" s="4"/>
       <c r="H12" s="4" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="I12" s="4"/>
       <c r="J12" s="4"/>
@@ -871,13 +781,13 @@
     </row>
     <row r="14" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="3" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B14" s="8"/>
     </row>
     <row r="15" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="3" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B15" s="9"/>
       <c r="C15" s="9"/>
@@ -886,105 +796,101 @@
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="E16" s="11"/>
     </row>
     <row r="17" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="12" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B17" s="12" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C17" s="12" t="s">
         <v>1</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="G17" s="13" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="H17" s="13" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="I17" s="3" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="J17" s="3" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="K17" s="3" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="L17" s="3" t="s">
         <v>7</v>
       </c>
       <c r="M17" s="14" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="O17" s="14"/>
       <c r="P17" s="14"/>
       <c r="Q17" s="14"/>
-      <c r="AMM17" s="1"/>
-      <c r="AMN17" s="1"/>
     </row>
     <row r="18" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="E18" s="8" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="F18" s="8" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="G18" s="15"/>
       <c r="H18" s="16"/>
       <c r="I18" s="1" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="J18" s="5" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="L18" s="5" t="s">
         <v>11</v>
       </c>
       <c r="M18" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="AMM18" s="1"/>
-      <c r="AMN18" s="1"/>
+        <v>33</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="3" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B20" s="8"/>
       <c r="F20" s="8"/>
     </row>
     <row r="21" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="3" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B21" s="9"/>
       <c r="C21" s="9"/>
@@ -999,225 +905,215 @@
     </row>
     <row r="23" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="12" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B23" s="12" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C23" s="12" t="s">
         <v>1</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="G23" s="13" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="H23" s="13" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="I23" s="3" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="J23" s="3" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="K23" s="3" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="L23" s="3" t="s">
         <v>7</v>
       </c>
       <c r="M23" s="14" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="N23" s="14" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="O23" s="14"/>
       <c r="P23" s="14"/>
       <c r="Q23" s="14"/>
-      <c r="AMM23" s="1"/>
-      <c r="AMN23" s="1"/>
     </row>
     <row r="24" customFormat="false" ht="150.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C24" s="8" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="E24" s="8" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="F24" s="8" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="G24" s="15"/>
       <c r="H24" s="16" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="J24" s="5" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="K24" s="1" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="L24" s="5" t="s">
         <v>11</v>
       </c>
       <c r="M24" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="N24" s="15" t="n">
         <v>9999</v>
       </c>
-      <c r="AMM24" s="1"/>
-      <c r="AMN24" s="1"/>
     </row>
     <row r="25" customFormat="false" ht="150.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B25" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D25" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="E25" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="F25" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="H25" s="16" t="s">
         <v>58</v>
       </c>
-      <c r="B25" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="D25" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="E25" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="F25" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="H25" s="16" t="s">
-        <v>56</v>
-      </c>
       <c r="I25" s="1" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="J25" s="5" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="K25" s="1" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="L25" s="5" t="s">
         <v>11</v>
       </c>
       <c r="M25" s="1" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="N25" s="15" t="n">
         <v>1111</v>
       </c>
-      <c r="AMM25" s="1"/>
-      <c r="AMN25" s="1"/>
     </row>
     <row r="26" customFormat="false" ht="58.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="E26" s="8" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="F26" s="8" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="G26" s="17" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="J26" s="5" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="K26" s="1" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="L26" s="5" t="s">
         <v>11</v>
       </c>
       <c r="M26" s="1" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="N26" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="AMM26" s="1"/>
-      <c r="AMN26" s="1"/>
     </row>
     <row r="27" customFormat="false" ht="58.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B27" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D27" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="E27" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="F27" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="G27" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="B27" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="D27" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="E27" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="F27" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="G27" s="17" t="s">
-        <v>65</v>
-      </c>
       <c r="I27" s="1" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="J27" s="5" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="K27" s="1" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="L27" s="5" t="s">
         <v>11</v>
       </c>
       <c r="M27" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="N27" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="AMM27" s="1"/>
-      <c r="AMN27" s="1"/>
     </row>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>

</xml_diff>

<commit_message>
BIS-1002: Fixed xls export test data
</commit_message>
<xml_diff>
--- a/server-application-server/sourceTest/java/ch/ethz/sis/openbis/generic/server/xls/export/resources/export-sample-with-referred-types.xlsx
+++ b/server-application-server/sourceTest/java/ch/ethz/sis/openbis/generic/server/xls/export/resources/export-sample-with-referred-types.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="74">
   <si>
     <t xml:space="preserve">SAMPLE_TYPE</t>
   </si>
@@ -92,6 +92,9 @@
   </si>
   <si>
     <t xml:space="preserve">Pattern Type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Internal Assignment</t>
   </si>
   <si>
     <t xml:space="preserve">$NAME</t>
@@ -306,6 +309,14 @@
     </font>
     <font>
       <b val="true"/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
       <sz val="13"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
@@ -323,14 +334,6 @@
     <font>
       <b val="true"/>
       <sz val="14"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -386,7 +389,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -415,6 +418,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -423,11 +430,11 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -439,11 +446,11 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -479,10 +486,10 @@
   <dimension ref="A1:Q1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N13" activeCellId="0" sqref="N13"/>
+      <selection pane="topLeft" activeCell="O11" activeCellId="0" sqref="O11:O12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.51953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.5234375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="38.68"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="42.5"/>
@@ -587,29 +594,32 @@
       <c r="N4" s="6" t="s">
         <v>23</v>
       </c>
+      <c r="O4" s="7" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>10</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G5" s="4"/>
       <c r="H5" s="4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="I5" s="4"/>
       <c r="J5" s="4"/>
@@ -619,29 +629,32 @@
       <c r="L5" s="4" t="s">
         <v>10</v>
       </c>
+      <c r="O5" s="4" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>10</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G6" s="4"/>
       <c r="H6" s="4" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="I6" s="4"/>
       <c r="J6" s="4"/>
@@ -651,6 +664,9 @@
       <c r="L6" s="4" t="s">
         <v>10</v>
       </c>
+      <c r="O6" s="4" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
@@ -682,10 +698,10 @@
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>10</v>
@@ -742,333 +758,339 @@
       <c r="N11" s="6" t="s">
         <v>23</v>
       </c>
+      <c r="O11" s="7" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>10</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G12" s="4"/>
       <c r="H12" s="4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="I12" s="4"/>
       <c r="J12" s="4"/>
       <c r="K12" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="L12" s="7" t="s">
+      <c r="L12" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="O12" s="4" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="3"/>
-      <c r="B13" s="8"/>
+      <c r="B13" s="9"/>
     </row>
     <row r="14" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="B14" s="8"/>
+        <v>35</v>
+      </c>
+      <c r="B14" s="9"/>
     </row>
     <row r="15" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="B15" s="9"/>
-      <c r="C15" s="9"/>
-      <c r="D15" s="9"/>
-      <c r="E15" s="10"/>
+        <v>36</v>
+      </c>
+      <c r="B15" s="10"/>
+      <c r="C15" s="10"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="11"/>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="E16" s="11"/>
+        <v>33</v>
+      </c>
+      <c r="E16" s="12"/>
     </row>
     <row r="17" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="B17" s="12" t="s">
+      <c r="A17" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="C17" s="12" t="s">
+      <c r="B17" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="C17" s="13" t="s">
         <v>1</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="G17" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="H17" s="13" t="s">
+      <c r="G17" s="14" t="s">
         <v>42</v>
       </c>
+      <c r="H17" s="14" t="s">
+        <v>43</v>
+      </c>
       <c r="I17" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="J17" s="3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="K17" s="3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="L17" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="M17" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="O17" s="14"/>
-      <c r="P17" s="14"/>
-      <c r="Q17" s="14"/>
+      <c r="M17" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="O17" s="15"/>
+      <c r="P17" s="15"/>
+      <c r="Q17" s="15"/>
     </row>
     <row r="18" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="B18" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="C18" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="D18" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="E18" s="8" t="s">
+      <c r="B18" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="F18" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="G18" s="15"/>
-      <c r="H18" s="16"/>
+      <c r="C18" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="D18" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="E18" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="F18" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="G18" s="16"/>
+      <c r="H18" s="17"/>
       <c r="I18" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="J18" s="5" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="L18" s="5" t="s">
         <v>11</v>
       </c>
       <c r="M18" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="B20" s="8"/>
-      <c r="F20" s="8"/>
+        <v>35</v>
+      </c>
+      <c r="B20" s="9"/>
+      <c r="F20" s="9"/>
     </row>
     <row r="21" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="B21" s="9"/>
-      <c r="C21" s="9"/>
-      <c r="D21" s="9"/>
-      <c r="E21" s="10"/>
+        <v>36</v>
+      </c>
+      <c r="B21" s="10"/>
+      <c r="C21" s="10"/>
+      <c r="D21" s="10"/>
+      <c r="E21" s="11"/>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E22" s="11"/>
+      <c r="E22" s="12"/>
     </row>
     <row r="23" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="B23" s="12" t="s">
+      <c r="A23" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="C23" s="12" t="s">
+      <c r="B23" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="C23" s="13" t="s">
         <v>1</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="G23" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="H23" s="13" t="s">
+      <c r="G23" s="14" t="s">
         <v>42</v>
       </c>
+      <c r="H23" s="14" t="s">
+        <v>43</v>
+      </c>
       <c r="I23" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="J23" s="3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="K23" s="3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="L23" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="M23" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="N23" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="O23" s="14"/>
-      <c r="P23" s="14"/>
-      <c r="Q23" s="14"/>
+      <c r="M23" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="N23" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="O23" s="15"/>
+      <c r="P23" s="15"/>
+      <c r="Q23" s="15"/>
     </row>
     <row r="24" customFormat="false" ht="150.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B24" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="C24" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="D24" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="E24" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="F24" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="G24" s="16"/>
+      <c r="H24" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="I24" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="J24" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="K24" s="1" t="s">
         <v>52</v>
-      </c>
-      <c r="B24" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="C24" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="D24" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="E24" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="F24" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="G24" s="15"/>
-      <c r="H24" s="16" t="s">
-        <v>58</v>
-      </c>
-      <c r="I24" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="J24" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="K24" s="1" t="s">
-        <v>51</v>
       </c>
       <c r="L24" s="5" t="s">
         <v>11</v>
       </c>
       <c r="M24" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="N24" s="15" t="n">
+        <v>60</v>
+      </c>
+      <c r="N24" s="16" t="n">
         <v>9999</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="150.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="B25" s="8" t="s">
         <v>61</v>
       </c>
+      <c r="B25" s="9" t="s">
+        <v>62</v>
+      </c>
       <c r="C25" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="D25" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="E25" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="D25" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="F25" s="8" t="s">
+      <c r="E25" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="H25" s="16" t="s">
+      <c r="F25" s="9" t="s">
         <v>58</v>
       </c>
+      <c r="H25" s="17" t="s">
+        <v>59</v>
+      </c>
       <c r="I25" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="J25" s="5" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="K25" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="L25" s="5" t="s">
         <v>11</v>
       </c>
       <c r="M25" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="N25" s="15" t="n">
+        <v>64</v>
+      </c>
+      <c r="N25" s="16" t="n">
         <v>1111</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="58.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="B26" s="8" t="s">
         <v>65</v>
       </c>
+      <c r="B26" s="9" t="s">
+        <v>66</v>
+      </c>
       <c r="C26" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="D26" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="E26" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="D26" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="F26" s="8" t="s">
+      <c r="E26" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="G26" s="17" t="s">
-        <v>67</v>
+      <c r="F26" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="G26" s="18" t="s">
+        <v>68</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="J26" s="5" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="K26" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="L26" s="5" t="s">
         <v>11</v>
       </c>
       <c r="M26" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="N26" s="1" t="n">
         <v>1</v>
@@ -1076,40 +1098,40 @@
     </row>
     <row r="27" customFormat="false" ht="58.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="B27" s="8" t="s">
         <v>70</v>
       </c>
+      <c r="B27" s="9" t="s">
+        <v>71</v>
+      </c>
       <c r="C27" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="D27" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="E27" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="D27" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="F27" s="8" t="s">
+      <c r="E27" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="G27" s="17" t="s">
-        <v>67</v>
+      <c r="F27" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="G27" s="18" t="s">
+        <v>68</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="J27" s="5" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="K27" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="L27" s="5" t="s">
         <v>11</v>
       </c>
       <c r="M27" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="N27" s="1" t="n">
         <v>2</v>

</xml_diff>